<commit_message>
Updates to fit workbook.
</commit_message>
<xml_diff>
--- a/OtherMaterials/DatasetFitsWorkbook.xlsx
+++ b/OtherMaterials/DatasetFitsWorkbook.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34814FBC-8E9F-D04C-BE02-18C1C7E1A165}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="35680" windowHeight="19380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Do all grid jobs with default Tc and Tvw time randomization</t>
   </si>
@@ -71,9 +72,6 @@
     <t>Pileup energy scan</t>
   </si>
   <si>
-    <t>CBO envelope checks</t>
-  </si>
-  <si>
     <t>Fixed k_loss scan</t>
   </si>
   <si>
@@ -86,9 +84,6 @@
     <t>maybe just do on-off with this</t>
   </si>
   <si>
-    <t>station 12/18, fixed parameters, different functional form</t>
-  </si>
-  <si>
     <t>Don't necessarily do all fits for all datasets - in some cases one should be enough</t>
   </si>
   <si>
@@ -98,15 +93,122 @@
     <t>fits done</t>
   </si>
   <si>
-    <t>grid jobs going or done</t>
+    <t>Lost muons on/off</t>
+  </si>
+  <si>
+    <t>Toy MC randomization comparison with VW randomization</t>
+  </si>
+  <si>
+    <t>2 grid jobs held and resubmitted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">take as my error more than 1 sigma due to unknown gain issue </t>
+  </si>
+  <si>
+    <t>use plots from fixed cbo tau</t>
+  </si>
+  <si>
+    <t>Plots to make</t>
+  </si>
+  <si>
+    <t>dataset combined lost muon fractions</t>
+  </si>
+  <si>
+    <t>other dataset combination plots</t>
+  </si>
+  <si>
+    <t>use plots from fixed cbo A A</t>
+  </si>
+  <si>
+    <t>correlation matrices</t>
+  </si>
+  <si>
+    <t>pileup spectra plots</t>
+  </si>
+  <si>
+    <t>Pileup deadtime scan</t>
+  </si>
+  <si>
+    <t>Make plots and fits from slide 27 of Elba talk</t>
+  </si>
+  <si>
+    <t>g-2 period scan</t>
+  </si>
+  <si>
+    <t>muon lifetime scan</t>
+  </si>
+  <si>
+    <t>Energy threshold scan</t>
+  </si>
+  <si>
+    <t>FFTs and residual plots (careful with hardcoded lines)</t>
+  </si>
+  <si>
+    <t>Fit end scans</t>
+  </si>
+  <si>
+    <t>Other things to do/ think about/ argue away</t>
+  </si>
+  <si>
+    <t>Gain - short term double pulse</t>
+  </si>
+  <si>
+    <t>Gain - unseen gain changes</t>
+  </si>
+  <si>
+    <t>Fit start scan comparison of pileup time shifted data</t>
+  </si>
+  <si>
+    <t>CBO frequency</t>
+  </si>
+  <si>
+    <t>station 12/18, vary fixed parameters</t>
+  </si>
+  <si>
+    <t>CBO envelope</t>
+  </si>
+  <si>
+    <t>different functional forms</t>
+  </si>
+  <si>
+    <t>Bunch number analysis</t>
+  </si>
+  <si>
+    <t>Row number analysis</t>
+  </si>
+  <si>
+    <t>Pileup gap time scan</t>
+  </si>
+  <si>
+    <t>grid jobs submitted, going, or done</t>
+  </si>
+  <si>
+    <t>ready to be fit</t>
+  </si>
+  <si>
+    <t>how important is this actually?</t>
+  </si>
+  <si>
+    <t>hadding</t>
+  </si>
+  <si>
+    <t>use plots from fixed cbo phases amps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -146,10 +248,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,6 +263,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -426,57 +533,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.5" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="49.1640625" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" customWidth="1"/>
-    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" customWidth="1"/>
+    <col min="10" max="12" width="40" customWidth="1"/>
+    <col min="13" max="13" width="49.1640625" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" customWidth="1"/>
+    <col min="15" max="15" width="57.1640625" customWidth="1"/>
+    <col min="16" max="16" width="28.6640625" customWidth="1"/>
+    <col min="17" max="17" width="26.5" customWidth="1"/>
+    <col min="18" max="18" width="28.6640625" customWidth="1"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="20" width="19.83203125" customWidth="1"/>
+    <col min="21" max="21" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -490,62 +602,216 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" t="s">
         <v>14</v>
       </c>
-      <c r="J6" t="s">
+      <c r="P6" t="s">
         <v>15</v>
       </c>
-      <c r="K6" t="s">
+      <c r="Q6" t="s">
         <v>16</v>
       </c>
-      <c r="L6" t="s">
+      <c r="R6" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" t="s">
+        <v>35</v>
+      </c>
+      <c r="U6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" t="s">
         <v>17</v>
       </c>
-      <c r="M6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="Q7" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="H8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to fit workbook and added high kick tracker model figures.
</commit_message>
<xml_diff>
--- a/OtherMaterials/DatasetFitsWorkbook.xlsx
+++ b/OtherMaterials/DatasetFitsWorkbook.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/GraduationRequirements/Dissertation/OtherMaterials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24836968-84BB-2744-BC88-C210C791A943}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="840" yWindow="880" windowWidth="34980" windowHeight="19600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
     <t>Do all grid jobs with default Tc and Tvw time randomization</t>
   </si>
@@ -188,9 +189,6 @@
     <t>Bunch number fits</t>
   </si>
   <si>
-    <t>Don't spend too much time on this, maybe only do it for the Endgame</t>
-  </si>
-  <si>
     <t>3500 MeV cut for pileup plots</t>
   </si>
   <si>
@@ -200,13 +198,61 @@
     <t>use plots from 9d fits</t>
   </si>
   <si>
-    <t>maybe just do on-off-twice with this</t>
+    <t>maybe just do on-off-twice with this - maybe skip this entirely</t>
+  </si>
+  <si>
+    <t>grid jobs submitted for on-off-twice</t>
+  </si>
+  <si>
+    <t>note to keep in mind</t>
+  </si>
+  <si>
+    <t>move lost muons and single iteration highkick stuff over to thesis directory</t>
+  </si>
+  <si>
+    <t>with - without</t>
+  </si>
+  <si>
+    <t>-31.4 ppb</t>
+  </si>
+  <si>
+    <t>-45.7 ppb</t>
+  </si>
+  <si>
+    <t>-6.1 ppb</t>
+  </si>
+  <si>
+    <t>1 sigma error: 0.338, slope = -3.5 ppb</t>
+  </si>
+  <si>
+    <t>1 sigma error: 0.170, slope = -18.3 ppb</t>
+  </si>
+  <si>
+    <t>1 sigma error: 0.038, slope = -2.6 ppb</t>
+  </si>
+  <si>
+    <t>grid/pnfs will be down Wednesday for a bit</t>
+  </si>
+  <si>
+    <t>Only use R plot for simplicity</t>
+  </si>
+  <si>
+    <t>use plots from all free</t>
+  </si>
+  <si>
+    <t>9 grid jobs in both cases were held and returned bad clusters hits files - not sure why and will probably need to rerun</t>
+  </si>
+  <si>
+    <t>maybe do a couple points on either side of the chi2 curve - find that curve or remake it - maybe do .5 and 1.5</t>
+  </si>
+  <si>
+    <t>sent grid jobs off for .5, 1.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -224,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +289,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -256,12 +308,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,17 +595,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C17" sqref="C17"/>
+      <selection pane="topRight" activeCell="K21" sqref="C21:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="1" max="1" width="68.5" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
@@ -565,8 +619,8 @@
     <col min="13" max="13" width="49.1640625" customWidth="1"/>
     <col min="14" max="14" width="20.83203125" customWidth="1"/>
     <col min="15" max="15" width="57.1640625" customWidth="1"/>
-    <col min="16" max="16" width="36.83203125" customWidth="1"/>
-    <col min="17" max="17" width="34.5" customWidth="1"/>
+    <col min="16" max="16" width="98" customWidth="1"/>
+    <col min="17" max="17" width="63.1640625" customWidth="1"/>
     <col min="18" max="18" width="28.6640625" customWidth="1"/>
     <col min="19" max="19" width="22" customWidth="1"/>
     <col min="20" max="20" width="28" customWidth="1"/>
@@ -591,6 +645,9 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
+      <c r="M3" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -603,280 +660,329 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="4"/>
+      <c r="P7" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>11</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>12</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I8" t="s">
         <v>13</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J8" t="s">
         <v>30</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K8" t="s">
         <v>47</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L8" t="s">
         <v>41</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M8" t="s">
         <v>43</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N8" t="s">
         <v>20</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O8" t="s">
         <v>14</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P8" t="s">
         <v>15</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q8" t="s">
         <v>16</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R8" t="s">
         <v>18</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S8" t="s">
         <v>32</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T8" t="s">
         <v>33</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U8" t="s">
         <v>34</v>
       </c>
-      <c r="V7" t="s">
+      <c r="V8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="J8" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
         <v>31</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L9" t="s">
         <v>42</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M9" t="s">
         <v>44</v>
       </c>
-      <c r="O8" t="s">
+      <c r="N9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O9" t="s">
         <v>22</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P9" t="s">
         <v>57</v>
       </c>
-      <c r="Q8" t="s">
-        <v>57</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="Q9" t="s">
+        <v>56</v>
+      </c>
+      <c r="R9" t="s">
         <v>50</v>
       </c>
-      <c r="V8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>49</v>
+      <c r="V9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E10" s="4"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
+      <c r="N10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="V10" s="2" t="s">
-        <v>49</v>
+      <c r="V10" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="4"/>
+        <v>51</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="K11" s="1"/>
+      <c r="N11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="V11" s="2" t="s">
-        <v>49</v>
+      <c r="V11" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="N12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="V12" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to fit workbook and lost muon comparison workbook.
</commit_message>
<xml_diff>
--- a/OtherMaterials/DatasetFitsWorkbook.xlsx
+++ b/OtherMaterials/DatasetFitsWorkbook.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67D0CB1-B63B-6F4B-8D77-40F9D275C1CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CEC736-8816-E440-B954-DEBFE23ED6A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="460" windowWidth="36800" windowHeight="20260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="111">
   <si>
     <t>Do all grid jobs with default Tc and Tvw time randomization</t>
   </si>
@@ -198,9 +198,6 @@
     <t>use plots from all free</t>
   </si>
   <si>
-    <t>maybe skip this entirely</t>
-  </si>
-  <si>
     <t>Gain - unseen gain changes - omit and study after thesis</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>I think for this error I'll need to show the plots I have and then calculate the systematic error slightly differently to how I was planning - mention extraneous points but still show that the slope is flatter than in the T method - take uncertainties from personal communication with Anna or with width of T method curve - final error is still small</t>
   </si>
   <si>
-    <t>Endgame dataset has the most lost muons and the largest fraction of lost muons, that combined with the negligible errors for the different lost muon subractions means that I should be able to just take the Endgame results</t>
-  </si>
-  <si>
     <t>STDP</t>
   </si>
   <si>
@@ -279,9 +273,6 @@
     <t>-40.1 ppb</t>
   </si>
   <si>
-    <t>my only worry here is that the lost muons on/off column for the various datasets is a lot larger for the non-endgame datasets surprisingly so I might want to do it for one of those</t>
-  </si>
-  <si>
     <t>1 sigma error: 0.697, slope = -7.1 ppb</t>
   </si>
   <si>
@@ -312,9 +303,6 @@
     <t>8 ppb</t>
   </si>
   <si>
-    <t>For fit end scans don't worry about spurious points as long as trends look stable and the R, A, phi and chi2 plots looks good.</t>
-  </si>
-  <si>
     <t>Not sure what to do about the different values between NA2 and sigmaR, 1660 vs 1700</t>
   </si>
   <si>
@@ -354,16 +342,25 @@
     <t>conservative / aggressive estimates of the error</t>
   </si>
   <si>
-    <t>look into these numbers again</t>
-  </si>
-  <si>
     <t>Put in favorite plots and numbers as is and then look and see what all the numbers look like in the thesis at the end of the day and potentially drop a point.</t>
   </si>
   <si>
     <t>Maybe just try to argue it away somehow - ultimately what's most important is sigmaR. There's some variation in sigmaR too though unfortunately. Probably show plots from a single dataset.</t>
   </si>
   <si>
-    <t xml:space="preserve">Put in kawall bands on R. </t>
+    <t>Some bug in the bin width scanning code - ratio fits are bad, T method fits are different even with the same bin width as compared to the single iter fits</t>
+  </si>
+  <si>
+    <t>Endgame dataset has the most lost muons and the largest fraction of lost muons, that combined with the negligible errors for the different lost muon subractions means that I should be able to just take the Endgame results, 9d results also show negligible change</t>
+  </si>
+  <si>
+    <t>look into these numbers again - don't understant the large change in 9d compared to endgame - also didn't I find that the on off value was equal to the slope extrapolation?</t>
+  </si>
+  <si>
+    <t>Doesn't really tell me any more than the amplitude scans.</t>
+  </si>
+  <si>
+    <t>For fit end scans don't worry about spurious points since trends look stable and the R, A, phi and chi2 plots looks good.</t>
   </si>
 </sst>
 </file>
@@ -750,8 +747,8 @@
   <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D17" sqref="D17"/>
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,12 +766,13 @@
     <col min="11" max="12" width="40" customWidth="1"/>
     <col min="13" max="13" width="53" customWidth="1"/>
     <col min="14" max="14" width="49.1640625" customWidth="1"/>
-    <col min="15" max="15" width="20.83203125" customWidth="1"/>
+    <col min="15" max="15" width="35.83203125" customWidth="1"/>
     <col min="16" max="17" width="57.1640625" customWidth="1"/>
     <col min="18" max="18" width="70.6640625" customWidth="1"/>
     <col min="19" max="19" width="22.6640625" customWidth="1"/>
     <col min="20" max="20" width="30.1640625" style="2" customWidth="1"/>
-    <col min="21" max="22" width="28.6640625" customWidth="1"/>
+    <col min="21" max="21" width="36.6640625" customWidth="1"/>
+    <col min="22" max="22" width="28.6640625" customWidth="1"/>
     <col min="23" max="23" width="22" customWidth="1"/>
     <col min="24" max="24" width="28" customWidth="1"/>
     <col min="25" max="25" width="40.1640625" customWidth="1"/>
@@ -818,7 +816,7 @@
     </row>
     <row r="7" spans="1:26" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -860,10 +858,10 @@
         <v>39</v>
       </c>
       <c r="L9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N9" t="s">
         <v>38</v>
@@ -875,7 +873,7 @@
         <v>14</v>
       </c>
       <c r="Q9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R9" t="s">
         <v>15</v>
@@ -884,13 +882,13 @@
         <v>16</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U9" t="s">
         <v>18</v>
       </c>
       <c r="V9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="W9" t="s">
         <v>31</v>
@@ -907,16 +905,16 @@
     </row>
     <row r="10" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="N10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="O10" t="s">
         <v>47</v>
@@ -925,13 +923,10 @@
         <v>22</v>
       </c>
       <c r="Q10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R10" t="s">
-        <v>68</v>
-      </c>
-      <c r="S10" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="Z10" t="s">
         <v>54</v>
@@ -956,11 +951,11 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="O11" s="4" t="s">
         <v>48</v>
@@ -970,11 +965,11 @@
       </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S11" s="5"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
@@ -1005,11 +1000,11 @@
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>49</v>
@@ -1017,17 +1012,19 @@
       <c r="P12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Q12" s="5"/>
+      <c r="Q12" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="R12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S12" s="5"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="Z12" s="1" t="s">
         <v>23</v>
@@ -1052,11 +1049,11 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="O13" s="4" t="s">
         <v>50</v>
@@ -1065,14 +1062,14 @@
         <v>53</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S13" s="5"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
@@ -1088,7 +1085,7 @@
         <v>-17.543299999999999</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>41</v>
@@ -1101,25 +1098,25 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q14" s="5"/>
       <c r="R14" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S14" s="5"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
@@ -1127,132 +1124,133 @@
     </row>
     <row r="15" spans="1:26" s="7" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="Q15" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="T15" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="R15" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="T15" s="6" t="s">
-        <v>80</v>
+      <c r="U15" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="Y15" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:26" s="7" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N16" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="P16" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q16" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="R16" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="T16" s="6"/>
       <c r="Y16" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" s="7" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" s="7" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T17" s="6"/>
-      <c r="Y17" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
     </row>
-    <row r="19" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="K26" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="K27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
     </row>
-    <row r="29" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>28</v>
       </c>
@@ -1283,42 +1281,42 @@
     </row>
     <row r="39" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on random seed section.
</commit_message>
<xml_diff>
--- a/OtherMaterials/DatasetFitsWorkbook.xlsx
+++ b/OtherMaterials/DatasetFitsWorkbook.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/GraduationRequirements/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75950D9-9E4B-EE45-BB62-1EC40E13ED92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="36800" windowHeight="20260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="107">
   <si>
     <t>Do all grid jobs with default Tc and Tvw time randomization</t>
   </si>
@@ -111,12 +110,6 @@
     <t>use plots from fixed cbo A A</t>
   </si>
   <si>
-    <t>correlation matrices</t>
-  </si>
-  <si>
-    <t>pileup spectra plots</t>
-  </si>
-  <si>
     <t>Pileup deadtime scan</t>
   </si>
   <si>
@@ -127,9 +120,6 @@
   </si>
   <si>
     <t>Energy threshold scan</t>
-  </si>
-  <si>
-    <t>FFTs and residual plots (careful with hardcoded lines)</t>
   </si>
   <si>
     <t>Fit end scans</t>
@@ -363,7 +353,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -381,7 +371,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,6 +402,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -425,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -454,6 +450,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,12 +736,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J26" sqref="J26"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -775,7 +772,7 @@
     <col min="26" max="26" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -784,12 +781,12 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
@@ -802,24 +799,24 @@
     </row>
     <row r="5" spans="1:26" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>2</v>
       </c>
@@ -833,7 +830,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
@@ -848,19 +845,19 @@
         <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9" t="s">
-        <v>79</v>
-      </c>
-      <c r="M9" t="s">
-        <v>80</v>
-      </c>
-      <c r="N9" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="O9" t="s">
         <v>20</v>
@@ -869,66 +866,66 @@
         <v>14</v>
       </c>
       <c r="Q9" t="s">
-        <v>65</v>
-      </c>
-      <c r="R9" t="s">
+        <v>62</v>
+      </c>
+      <c r="R9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="T9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="U9" t="s">
+      <c r="T9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="U9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="V9" t="s">
-        <v>61</v>
-      </c>
-      <c r="W9" t="s">
+      <c r="V9" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="W9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="X9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y9" t="s">
         <v>30</v>
       </c>
-      <c r="X9" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>32</v>
-      </c>
       <c r="Z9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="M10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="P10" t="s">
         <v>22</v>
       </c>
       <c r="Q10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Z10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>3</v>
       </c>
@@ -947,21 +944,21 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="O11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="S11" s="5"/>
       <c r="U11" s="1"/>
@@ -970,10 +967,10 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>4</v>
       </c>
@@ -981,10 +978,10 @@
         <v>-17.821400000000001</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -992,27 +989,27 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="O12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="Q12" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="S12" s="5"/>
       <c r="U12" s="1"/>
@@ -1020,13 +1017,13 @@
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="Z12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
@@ -1045,23 +1042,23 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="Q13" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="S13" s="5"/>
       <c r="U13" s="1"/>
@@ -1070,10 +1067,10 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -1081,10 +1078,10 @@
         <v>-17.543299999999999</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1094,21 +1091,21 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q14" s="5"/>
       <c r="R14" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="S14" s="5"/>
       <c r="U14" s="1"/>
@@ -1120,108 +1117,108 @@
     </row>
     <row r="15" spans="1:26" s="7" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E15" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="P15" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="P15" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="Q15" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S15" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="U15" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="Y15" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:26" s="7" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="O16" s="6"/>
       <c r="P16" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="Q16" s="6"/>
       <c r="R16" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="T16" s="6"/>
       <c r="Y16" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="7" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="T17" s="6"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
     </row>
-    <row r="19" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="7" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1230,7 +1227,7 @@
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
     </row>
-    <row r="29" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>24</v>
       </c>
@@ -1238,29 +1235,23 @@
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" s="7"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="7"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
@@ -1272,34 +1263,34 @@
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
     </row>
-    <row r="39" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Some change to dataset fit workbook.
</commit_message>
<xml_diff>
--- a/OtherMaterials/DatasetFitsWorkbook.xlsx
+++ b/OtherMaterials/DatasetFitsWorkbook.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -146,9 +146,6 @@
     <t>Bunch number fits</t>
   </si>
   <si>
-    <t>3500 MeV cut for pileup plots</t>
-  </si>
-  <si>
     <t>same R mean as without 2N CBO</t>
   </si>
   <si>
@@ -348,6 +345,9 @@
   </si>
   <si>
     <t>Gain - short term double pulse</t>
+  </si>
+  <si>
+    <t>maybe I should do more gain point fits</t>
   </si>
 </sst>
 </file>
@@ -739,9 +739,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,12 +804,12 @@
     </row>
     <row r="6" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -851,10 +851,10 @@
         <v>35</v>
       </c>
       <c r="L9" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="14" t="s">
         <v>76</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>77</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>34</v>
@@ -866,7 +866,7 @@
         <v>14</v>
       </c>
       <c r="Q9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R9" s="14" t="s">
         <v>15</v>
@@ -875,13 +875,13 @@
         <v>16</v>
       </c>
       <c r="T9" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U9" s="14" t="s">
         <v>18</v>
       </c>
       <c r="V9" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W9" s="14" t="s">
         <v>28</v>
@@ -898,31 +898,31 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P10" t="s">
         <v>22</v>
       </c>
       <c r="Q10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
@@ -944,21 +944,21 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S11" s="5"/>
       <c r="U11" s="1"/>
@@ -967,7 +967,7 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
@@ -978,7 +978,7 @@
         <v>-17.821400000000001</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>37</v>
@@ -989,27 +989,27 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S12" s="5"/>
       <c r="U12" s="1"/>
@@ -1017,7 +1017,7 @@
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Z12" s="1" t="s">
         <v>23</v>
@@ -1042,23 +1042,23 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S13" s="5"/>
       <c r="U13" s="1"/>
@@ -1067,7 +1067,7 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
@@ -1078,7 +1078,7 @@
         <v>-17.543299999999999</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>37</v>
@@ -1091,21 +1091,21 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="Q14" s="5"/>
       <c r="R14" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S14" s="5"/>
       <c r="U14" s="1"/>
@@ -1117,74 +1117,77 @@
     </row>
     <row r="15" spans="1:26" s="7" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q15" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="S15" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="R15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="S15" s="7" t="s">
-        <v>99</v>
-      </c>
       <c r="T15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U15" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Y15" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:26" s="7" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O16" s="6"/>
       <c r="P16" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q16" s="6"/>
       <c r="R16" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T16" s="6"/>
       <c r="Y16" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="7" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="R17" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="T17" s="6"/>
     </row>
@@ -1198,7 +1201,7 @@
     </row>
     <row r="20" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
@@ -1207,18 +1210,16 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="A22" s="6"/>
     </row>
     <row r="23" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="7" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1265,32 +1266,32 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>